<commit_message>
More updates on OS configuration. Fixes on Scheduletables. Started on kernel testsystem, again.
</commit_message>
<xml_diff>
--- a/scripts/req-os.xlsx
+++ b/scripts/req-os.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9114"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="465" windowWidth="27555" windowHeight="14025"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="575">
   <si>
     <t>id</t>
   </si>
@@ -916,12 +916,6 @@
   <si>
     <t>If ShutdownOS() is called and ShutdownHook() returns then the operating
 system shall disable all interrupts and enter an endless loop.</t>
-  </si>
-  <si>
-    <t>The Operating System shall provide the services DisableAllInterrupts(),
-EnableAllInterrupts(),  SuspendAllInterrupts(),  ResumeAllInterrupts()
-prior to calling StartOS() and after calling ShutdownOS(). (It is assumed that the
-static variables of these functions are initialized).</t>
   </si>
   <si>
     <t>The Operating System  shall provide the ability  to increment a software
@@ -2129,12 +2123,19 @@
   <si>
     <t>,3,4</t>
   </si>
+  <si>
+    <t>The Operating System shall provide the services DisableAllInterrupts(), EnableAllInterrupts(),  SuspendAllInterrupts(),  ResumeAllInterrupts()
+prior to calling StartOS() and after calling ShutdownOS(). (It is assumed that the static variables of these functions are initialized).</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2177,25 +2178,25 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2271,34 +2272,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1F497D" mc:Ignorable=""/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="EEECE1" mc:Ignorable=""/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="4F81BD" mc:Ignorable=""/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C0504D" mc:Ignorable=""/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="9BBB59" mc:Ignorable=""/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="8064A2" mc:Ignorable=""/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="4BACC6" mc:Ignorable=""/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="F79646" mc:Ignorable=""/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0000FF" mc:Ignorable=""/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="800080" mc:Ignorable=""/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -2335,7 +2336,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2370,7 +2370,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2452,7 +2451,7 @@
         <a:effectStyle>
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
+              <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
             </a:outerShdw>
@@ -2461,7 +2460,7 @@
         <a:effectStyle>
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
+              <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
@@ -2470,7 +2469,7 @@
         <a:effectStyle>
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
+              <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
@@ -2546,23 +2545,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="B194" sqref="B194"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="76.42578125" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="30">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2678,10 +2678,10 @@
         <v>288</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -2695,10 +2695,10 @@
         <v>288</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -2712,10 +2712,10 @@
         <v>288</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -2729,10 +2729,10 @@
         <v>288</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="60">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -2746,10 +2746,10 @@
         <v>288</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -2763,10 +2763,10 @@
         <v>288</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -2780,10 +2780,10 @@
         <v>288</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -2791,16 +2791,16 @@
         <v>283</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>288</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -2808,16 +2808,16 @@
         <v>283</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>288</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -2825,16 +2825,16 @@
         <v>283</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>288</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -2842,16 +2842,16 @@
         <v>283</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>288</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -2859,16 +2859,16 @@
         <v>283</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>288</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -2876,16 +2876,16 @@
         <v>283</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>288</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -2893,16 +2893,16 @@
         <v>283</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>288</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -2910,16 +2910,16 @@
         <v>283</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>288</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -2927,16 +2927,16 @@
         <v>283</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>288</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -2950,10 +2950,10 @@
         <v>288</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -2967,10 +2967,10 @@
         <v>288</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -2984,10 +2984,10 @@
         <v>288</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -3001,10 +3001,10 @@
         <v>288</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -3018,10 +3018,10 @@
         <v>288</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -3035,10 +3035,10 @@
         <v>288</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -3046,16 +3046,16 @@
         <v>283</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>288</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="45">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -3069,10 +3069,10 @@
         <v>288</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -3086,10 +3086,10 @@
         <v>288</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="45">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -3103,10 +3103,10 @@
         <v>288</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -3120,10 +3120,10 @@
         <v>288</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -3137,10 +3137,10 @@
         <v>288</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -3154,10 +3154,10 @@
         <v>288</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="45">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -3171,10 +3171,10 @@
         <v>288</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -3188,10 +3188,10 @@
         <v>288</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -3205,10 +3205,10 @@
         <v>288</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30">
       <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
@@ -3222,10 +3222,10 @@
         <v>288</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30">
       <c r="A40" s="1" t="s">
         <v>43</v>
       </c>
@@ -3239,10 +3239,10 @@
         <v>288</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="30">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -3256,10 +3256,10 @@
         <v>288</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="30">
       <c r="A42" s="1" t="s">
         <v>45</v>
       </c>
@@ -3273,10 +3273,10 @@
         <v>288</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30">
       <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
@@ -3290,10 +3290,10 @@
         <v>288</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30">
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
@@ -3307,10 +3307,10 @@
         <v>288</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="45">
       <c r="A45" s="1" t="s">
         <v>48</v>
       </c>
@@ -3324,10 +3324,10 @@
         <v>288</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="30">
       <c r="A46" s="1" t="s">
         <v>49</v>
       </c>
@@ -3341,10 +3341,10 @@
         <v>288</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
@@ -3358,10 +3358,10 @@
         <v>288</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="30">
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
@@ -3375,10 +3375,10 @@
         <v>288</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -3392,10 +3392,10 @@
         <v>288</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="45">
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
@@ -3409,10 +3409,10 @@
         <v>288</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="45">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
@@ -3426,10 +3426,10 @@
         <v>288</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="30">
       <c r="A52" s="1" t="s">
         <v>55</v>
       </c>
@@ -3443,10 +3443,10 @@
         <v>288</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="30">
       <c r="A53" s="1" t="s">
         <v>56</v>
       </c>
@@ -3460,15 +3460,15 @@
         <v>288</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="30">
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>288</v>
@@ -3477,10 +3477,10 @@
         <v>288</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="45">
       <c r="A55" s="1" t="s">
         <v>58</v>
       </c>
@@ -3494,10 +3494,10 @@
         <v>288</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="30">
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
@@ -3511,10 +3511,10 @@
         <v>288</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
         <v>60</v>
       </c>
@@ -3528,15 +3528,15 @@
         <v>288</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>288</v>
@@ -3545,15 +3545,15 @@
         <v>288</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="45">
       <c r="A59" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>288</v>
@@ -3562,15 +3562,15 @@
         <v>288</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="45">
       <c r="A60" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>288</v>
@@ -3579,15 +3579,15 @@
         <v>288</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30">
       <c r="A61" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>288</v>
@@ -3596,15 +3596,15 @@
         <v>288</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30">
       <c r="A62" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>288</v>
@@ -3613,10 +3613,10 @@
         <v>288</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="30">
       <c r="A63" s="1" t="s">
         <v>66</v>
       </c>
@@ -3624,21 +3624,21 @@
         <v>283</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>288</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="45">
       <c r="A64" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>283</v>
+        <v>574</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>288</v>
@@ -3647,15 +3647,15 @@
         <v>288</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="45">
       <c r="A65" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>288</v>
@@ -3664,15 +3664,15 @@
         <v>288</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="60">
       <c r="A66" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>288</v>
@@ -3681,10 +3681,10 @@
         <v>288</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="30">
       <c r="A67" s="1" t="s">
         <v>70</v>
       </c>
@@ -3698,15 +3698,15 @@
         <v>288</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="30">
       <c r="A68" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>288</v>
@@ -3715,10 +3715,10 @@
         <v>288</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="30">
       <c r="A69" s="1" t="s">
         <v>72</v>
       </c>
@@ -3732,10 +3732,10 @@
         <v>288</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="45">
       <c r="A70" s="1" t="s">
         <v>73</v>
       </c>
@@ -3749,10 +3749,10 @@
         <v>288</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="45">
       <c r="A71" s="1" t="s">
         <v>74</v>
       </c>
@@ -3766,10 +3766,10 @@
         <v>288</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="60">
       <c r="A72" s="1" t="s">
         <v>75</v>
       </c>
@@ -3783,10 +3783,10 @@
         <v>288</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" s="1" t="s">
         <v>76</v>
       </c>
@@ -3800,10 +3800,10 @@
         <v>288</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="45">
       <c r="A74" s="1" t="s">
         <v>77</v>
       </c>
@@ -3817,10 +3817,10 @@
         <v>288</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="30">
       <c r="A75" s="1" t="s">
         <v>78</v>
       </c>
@@ -3834,10 +3834,10 @@
         <v>288</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30">
       <c r="A76" s="1" t="s">
         <v>79</v>
       </c>
@@ -3851,10 +3851,10 @@
         <v>288</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30">
       <c r="A77" s="1" t="s">
         <v>80</v>
       </c>
@@ -3868,10 +3868,10 @@
         <v>288</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="30">
       <c r="A78" s="1" t="s">
         <v>81</v>
       </c>
@@ -3885,10 +3885,10 @@
         <v>288</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="30">
       <c r="A79" s="1" t="s">
         <v>82</v>
       </c>
@@ -3902,10 +3902,10 @@
         <v>288</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="45">
       <c r="A80" s="1" t="s">
         <v>83</v>
       </c>
@@ -3919,10 +3919,10 @@
         <v>288</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="45">
       <c r="A81" s="1" t="s">
         <v>84</v>
       </c>
@@ -3936,10 +3936,10 @@
         <v>288</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="30">
       <c r="A82" s="1" t="s">
         <v>85</v>
       </c>
@@ -3953,10 +3953,10 @@
         <v>288</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="45">
       <c r="A83" s="1" t="s">
         <v>86</v>
       </c>
@@ -3970,10 +3970,10 @@
         <v>288</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="45">
       <c r="A84" s="1" t="s">
         <v>87</v>
       </c>
@@ -3987,10 +3987,10 @@
         <v>288</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="30">
       <c r="A85" s="1" t="s">
         <v>88</v>
       </c>
@@ -4004,10 +4004,10 @@
         <v>288</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="30">
       <c r="A86" s="1" t="s">
         <v>89</v>
       </c>
@@ -4021,10 +4021,10 @@
         <v>288</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="30">
       <c r="A87" s="1" t="s">
         <v>90</v>
       </c>
@@ -4038,10 +4038,10 @@
         <v>288</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="45">
       <c r="A88" s="1" t="s">
         <v>91</v>
       </c>
@@ -4055,10 +4055,10 @@
         <v>288</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="30">
       <c r="A89" s="1" t="s">
         <v>92</v>
       </c>
@@ -4072,10 +4072,10 @@
         <v>288</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="30">
       <c r="A90" s="1" t="s">
         <v>93</v>
       </c>
@@ -4089,10 +4089,10 @@
         <v>288</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="30">
       <c r="A91" s="1" t="s">
         <v>94</v>
       </c>
@@ -4106,10 +4106,10 @@
         <v>288</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="30">
       <c r="A92" s="1" t="s">
         <v>95</v>
       </c>
@@ -4123,10 +4123,10 @@
         <v>288</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="30">
       <c r="A93" s="1" t="s">
         <v>96</v>
       </c>
@@ -4140,10 +4140,10 @@
         <v>288</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="30">
       <c r="A94" s="1" t="s">
         <v>97</v>
       </c>
@@ -4157,10 +4157,10 @@
         <v>288</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="30">
       <c r="A95" s="1" t="s">
         <v>98</v>
       </c>
@@ -4174,10 +4174,10 @@
         <v>288</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="30">
       <c r="A96" s="1" t="s">
         <v>99</v>
       </c>
@@ -4191,10 +4191,10 @@
         <v>288</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="30">
       <c r="A97" s="1" t="s">
         <v>100</v>
       </c>
@@ -4208,10 +4208,10 @@
         <v>288</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="45">
       <c r="A98" s="1" t="s">
         <v>101</v>
       </c>
@@ -4225,10 +4225,10 @@
         <v>288</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="45">
       <c r="A99" s="1" t="s">
         <v>102</v>
       </c>
@@ -4242,10 +4242,10 @@
         <v>288</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="30">
       <c r="A100" s="1" t="s">
         <v>103</v>
       </c>
@@ -4259,10 +4259,10 @@
         <v>288</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="30">
       <c r="A101" s="1" t="s">
         <v>104</v>
       </c>
@@ -4276,10 +4276,10 @@
         <v>288</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="30">
       <c r="A102" s="1" t="s">
         <v>105</v>
       </c>
@@ -4293,10 +4293,10 @@
         <v>288</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="60">
       <c r="A103" s="1" t="s">
         <v>106</v>
       </c>
@@ -4310,10 +4310,10 @@
         <v>288</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="45">
       <c r="A104" s="1" t="s">
         <v>107</v>
       </c>
@@ -4327,10 +4327,10 @@
         <v>288</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="45">
       <c r="A105" s="1" t="s">
         <v>108</v>
       </c>
@@ -4344,10 +4344,10 @@
         <v>288</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="60">
       <c r="A106" s="1" t="s">
         <v>109</v>
       </c>
@@ -4361,10 +4361,10 @@
         <v>288</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="45">
       <c r="A107" s="1" t="s">
         <v>110</v>
       </c>
@@ -4378,10 +4378,10 @@
         <v>288</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" s="1" t="s">
         <v>111</v>
       </c>
@@ -4395,10 +4395,10 @@
         <v>288</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="45">
       <c r="A109" s="1" t="s">
         <v>112</v>
       </c>
@@ -4412,10 +4412,10 @@
         <v>288</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
       <c r="A110" s="1" t="s">
         <v>113</v>
       </c>
@@ -4429,10 +4429,10 @@
         <v>288</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="45">
       <c r="A111" s="1" t="s">
         <v>114</v>
       </c>
@@ -4446,10 +4446,10 @@
         <v>288</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="45">
       <c r="A112" s="1" t="s">
         <v>115</v>
       </c>
@@ -4463,10 +4463,10 @@
         <v>288</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113" s="1" t="s">
         <v>116</v>
       </c>
@@ -4480,10 +4480,10 @@
         <v>288</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="60">
       <c r="A114" s="1" t="s">
         <v>117</v>
       </c>
@@ -4497,10 +4497,10 @@
         <v>288</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="30">
       <c r="A115" s="1" t="s">
         <v>118</v>
       </c>
@@ -4514,10 +4514,10 @@
         <v>288</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="60">
       <c r="A116" s="1" t="s">
         <v>119</v>
       </c>
@@ -4531,10 +4531,10 @@
         <v>288</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
       <c r="A117" s="1" t="s">
         <v>120</v>
       </c>
@@ -4548,10 +4548,10 @@
         <v>288</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="30">
       <c r="A118" s="1" t="s">
         <v>121</v>
       </c>
@@ -4565,10 +4565,10 @@
         <v>288</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
       <c r="A119" s="1" t="s">
         <v>122</v>
       </c>
@@ -4582,10 +4582,10 @@
         <v>288</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="45">
       <c r="A120" s="1" t="s">
         <v>123</v>
       </c>
@@ -4599,10 +4599,10 @@
         <v>288</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="45">
       <c r="A121" s="1" t="s">
         <v>124</v>
       </c>
@@ -4616,10 +4616,10 @@
         <v>288</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="30">
       <c r="A122" s="1" t="s">
         <v>125</v>
       </c>
@@ -4633,10 +4633,10 @@
         <v>288</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="45">
       <c r="A123" s="1" t="s">
         <v>126</v>
       </c>
@@ -4650,10 +4650,10 @@
         <v>288</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="30">
       <c r="A124" s="1" t="s">
         <v>127</v>
       </c>
@@ -4667,10 +4667,10 @@
         <v>288</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="30">
       <c r="A125" s="1" t="s">
         <v>128</v>
       </c>
@@ -4684,10 +4684,10 @@
         <v>288</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="30">
       <c r="A126" s="1" t="s">
         <v>129</v>
       </c>
@@ -4701,10 +4701,10 @@
         <v>288</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="30">
       <c r="A127" s="1" t="s">
         <v>130</v>
       </c>
@@ -4718,10 +4718,10 @@
         <v>288</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="45">
       <c r="A128" s="1" t="s">
         <v>131</v>
       </c>
@@ -4735,10 +4735,10 @@
         <v>288</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="30">
       <c r="A129" s="1" t="s">
         <v>132</v>
       </c>
@@ -4752,10 +4752,10 @@
         <v>288</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
       <c r="A130" s="1" t="s">
         <v>133</v>
       </c>
@@ -4769,10 +4769,10 @@
         <v>288</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="30">
       <c r="A131" s="1" t="s">
         <v>134</v>
       </c>
@@ -4786,10 +4786,10 @@
         <v>288</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="30">
       <c r="A132" s="1" t="s">
         <v>135</v>
       </c>
@@ -4803,10 +4803,10 @@
         <v>288</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="45">
       <c r="A133" s="1" t="s">
         <v>136</v>
       </c>
@@ -4820,10 +4820,10 @@
         <v>288</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="30">
       <c r="A134" s="1" t="s">
         <v>137</v>
       </c>
@@ -4837,10 +4837,10 @@
         <v>288</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
       <c r="A135" s="1" t="s">
         <v>138</v>
       </c>
@@ -4854,10 +4854,10 @@
         <v>288</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
       <c r="A136" s="1" t="s">
         <v>139</v>
       </c>
@@ -4871,10 +4871,10 @@
         <v>288</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
       <c r="A137" s="1" t="s">
         <v>140</v>
       </c>
@@ -4888,10 +4888,10 @@
         <v>288</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="30">
       <c r="A138" s="1" t="s">
         <v>141</v>
       </c>
@@ -4905,10 +4905,10 @@
         <v>288</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="30">
       <c r="A139" s="1" t="s">
         <v>142</v>
       </c>
@@ -4916,16 +4916,16 @@
         <v>283</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="30">
       <c r="A140" s="1" t="s">
         <v>143</v>
       </c>
@@ -4933,16 +4933,16 @@
         <v>283</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="30">
       <c r="A141" s="1" t="s">
         <v>144</v>
       </c>
@@ -4956,10 +4956,10 @@
         <v>288</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="45">
       <c r="A142" s="1" t="s">
         <v>145</v>
       </c>
@@ -4973,10 +4973,10 @@
         <v>288</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="30">
       <c r="A143" s="1" t="s">
         <v>146</v>
       </c>
@@ -4990,10 +4990,10 @@
         <v>288</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="30">
       <c r="A144" s="1" t="s">
         <v>147</v>
       </c>
@@ -5007,10 +5007,10 @@
         <v>288</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="45">
       <c r="A145" s="1" t="s">
         <v>148</v>
       </c>
@@ -5024,10 +5024,10 @@
         <v>288</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="45">
       <c r="A146" s="1" t="s">
         <v>149</v>
       </c>
@@ -5041,10 +5041,10 @@
         <v>288</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="30">
       <c r="A147" s="1" t="s">
         <v>150</v>
       </c>
@@ -5058,10 +5058,10 @@
         <v>288</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="60">
       <c r="A148" s="1" t="s">
         <v>151</v>
       </c>
@@ -5075,10 +5075,10 @@
         <v>288</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
       <c r="A149" s="1" t="s">
         <v>152</v>
       </c>
@@ -5092,10 +5092,10 @@
         <v>288</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="30">
       <c r="A150" s="1" t="s">
         <v>153</v>
       </c>
@@ -5109,10 +5109,10 @@
         <v>288</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="30">
       <c r="A151" s="1" t="s">
         <v>154</v>
       </c>
@@ -5126,10 +5126,10 @@
         <v>288</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="30">
       <c r="A152" s="1" t="s">
         <v>155</v>
       </c>
@@ -5143,10 +5143,10 @@
         <v>288</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="30">
       <c r="A153" s="1" t="s">
         <v>156</v>
       </c>
@@ -5160,10 +5160,10 @@
         <v>288</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="30">
       <c r="A154" s="1" t="s">
         <v>157</v>
       </c>
@@ -5177,10 +5177,10 @@
         <v>288</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="45">
       <c r="A155" s="1" t="s">
         <v>158</v>
       </c>
@@ -5194,10 +5194,10 @@
         <v>288</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
       <c r="A156" s="1" t="s">
         <v>159</v>
       </c>
@@ -5211,10 +5211,10 @@
         <v>288</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" ht="60">
       <c r="A157" s="1" t="s">
         <v>160</v>
       </c>
@@ -5228,10 +5228,10 @@
         <v>288</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="30">
       <c r="A158" s="1" t="s">
         <v>161</v>
       </c>
@@ -5245,10 +5245,10 @@
         <v>288</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="45">
       <c r="A159" s="1" t="s">
         <v>162</v>
       </c>
@@ -5262,10 +5262,10 @@
         <v>288</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" ht="45">
       <c r="A160" s="1" t="s">
         <v>163</v>
       </c>
@@ -5279,10 +5279,10 @@
         <v>288</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="30">
       <c r="A161" s="1" t="s">
         <v>164</v>
       </c>
@@ -5296,10 +5296,10 @@
         <v>288</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="30">
       <c r="A162" s="1" t="s">
         <v>165</v>
       </c>
@@ -5313,10 +5313,10 @@
         <v>288</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" ht="30">
       <c r="A163" s="1" t="s">
         <v>166</v>
       </c>
@@ -5330,10 +5330,10 @@
         <v>288</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" ht="30">
       <c r="A164" s="1" t="s">
         <v>167</v>
       </c>
@@ -5347,10 +5347,10 @@
         <v>288</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" ht="30">
       <c r="A165" s="1" t="s">
         <v>168</v>
       </c>
@@ -5364,10 +5364,10 @@
         <v>288</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" ht="30">
       <c r="A166" s="1" t="s">
         <v>169</v>
       </c>
@@ -5381,10 +5381,10 @@
         <v>288</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" ht="30">
       <c r="A167" s="1" t="s">
         <v>170</v>
       </c>
@@ -5398,10 +5398,10 @@
         <v>288</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" ht="30">
       <c r="A168" s="1" t="s">
         <v>171</v>
       </c>
@@ -5415,10 +5415,10 @@
         <v>288</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="30">
       <c r="A169" s="1" t="s">
         <v>172</v>
       </c>
@@ -5432,10 +5432,10 @@
         <v>288</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="45">
       <c r="A170" s="1" t="s">
         <v>173</v>
       </c>
@@ -5449,10 +5449,10 @@
         <v>288</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" ht="30">
       <c r="A171" s="1" t="s">
         <v>174</v>
       </c>
@@ -5466,10 +5466,10 @@
         <v>288</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" ht="30">
       <c r="A172" s="1" t="s">
         <v>175</v>
       </c>
@@ -5483,10 +5483,10 @@
         <v>288</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" ht="45">
       <c r="A173" s="1" t="s">
         <v>176</v>
       </c>
@@ -5500,10 +5500,10 @@
         <v>288</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" ht="30">
       <c r="A174" s="1" t="s">
         <v>177</v>
       </c>
@@ -5517,10 +5517,10 @@
         <v>288</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" ht="30">
       <c r="A175" s="1" t="s">
         <v>178</v>
       </c>
@@ -5534,10 +5534,10 @@
         <v>288</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" ht="45">
       <c r="A176" s="1" t="s">
         <v>179</v>
       </c>
@@ -5551,10 +5551,10 @@
         <v>288</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" ht="30">
       <c r="A177" s="1" t="s">
         <v>180</v>
       </c>
@@ -5568,10 +5568,10 @@
         <v>288</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="45">
       <c r="A178" s="1" t="s">
         <v>181</v>
       </c>
@@ -5585,10 +5585,10 @@
         <v>288</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="45">
       <c r="A179" s="1" t="s">
         <v>182</v>
       </c>
@@ -5602,10 +5602,10 @@
         <v>288</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
       <c r="A180" s="1" t="s">
         <v>183</v>
       </c>
@@ -5619,10 +5619,10 @@
         <v>288</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" ht="30">
       <c r="A181" s="1" t="s">
         <v>184</v>
       </c>
@@ -5636,10 +5636,10 @@
         <v>288</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="30">
       <c r="A182" s="1" t="s">
         <v>185</v>
       </c>
@@ -5653,10 +5653,10 @@
         <v>288</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" ht="45">
       <c r="A183" s="1" t="s">
         <v>186</v>
       </c>
@@ -5670,10 +5670,10 @@
         <v>288</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
       <c r="A184" s="1" t="s">
         <v>187</v>
       </c>
@@ -5687,10 +5687,10 @@
         <v>288</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" ht="30">
       <c r="A185" s="1" t="s">
         <v>188</v>
       </c>
@@ -5704,10 +5704,10 @@
         <v>288</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" ht="45">
       <c r="A186" s="1" t="s">
         <v>189</v>
       </c>
@@ -5721,10 +5721,10 @@
         <v>288</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" ht="60">
       <c r="A187" s="1" t="s">
         <v>190</v>
       </c>
@@ -5738,10 +5738,10 @@
         <v>288</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" ht="45">
       <c r="A188" s="1" t="s">
         <v>191</v>
       </c>
@@ -5755,10 +5755,10 @@
         <v>288</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" ht="45">
       <c r="A189" s="1" t="s">
         <v>192</v>
       </c>
@@ -5772,10 +5772,10 @@
         <v>288</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" ht="60">
       <c r="A190" s="1" t="s">
         <v>193</v>
       </c>
@@ -5789,10 +5789,10 @@
         <v>288</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" ht="60">
       <c r="A191" s="1" t="s">
         <v>194</v>
       </c>
@@ -5806,10 +5806,10 @@
         <v>288</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
       <c r="A192" s="1" t="s">
         <v>195</v>
       </c>
@@ -5823,10 +5823,10 @@
         <v>288</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" ht="75">
       <c r="A193" s="1" t="s">
         <v>196</v>
       </c>
@@ -5840,10 +5840,10 @@
         <v>288</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" ht="45">
       <c r="A194" s="1" t="s">
         <v>197</v>
       </c>
@@ -5857,10 +5857,10 @@
         <v>288</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" ht="30">
       <c r="A195" s="1" t="s">
         <v>198</v>
       </c>
@@ -5874,10 +5874,10 @@
         <v>288</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" ht="60">
       <c r="A196" s="1" t="s">
         <v>199</v>
       </c>
@@ -5891,10 +5891,10 @@
         <v>288</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" ht="30">
       <c r="A197" s="1" t="s">
         <v>200</v>
       </c>
@@ -5908,10 +5908,10 @@
         <v>288</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
       <c r="A198" s="1" t="s">
         <v>201</v>
       </c>
@@ -5925,10 +5925,10 @@
         <v>288</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" ht="45">
       <c r="A199" s="1" t="s">
         <v>202</v>
       </c>
@@ -5942,10 +5942,10 @@
         <v>288</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" ht="30">
       <c r="A200" s="1" t="s">
         <v>203</v>
       </c>
@@ -5959,10 +5959,10 @@
         <v>288</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" ht="45">
       <c r="A201" s="1" t="s">
         <v>204</v>
       </c>
@@ -5976,10 +5976,10 @@
         <v>288</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" ht="45">
       <c r="A202" s="1" t="s">
         <v>205</v>
       </c>
@@ -5993,10 +5993,10 @@
         <v>288</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" ht="45">
       <c r="A203" s="1" t="s">
         <v>206</v>
       </c>
@@ -6010,10 +6010,10 @@
         <v>288</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" ht="45">
       <c r="A204" s="1" t="s">
         <v>207</v>
       </c>
@@ -6027,10 +6027,10 @@
         <v>288</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" ht="30">
       <c r="A205" s="1" t="s">
         <v>208</v>
       </c>
@@ -6044,10 +6044,10 @@
         <v>288</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" ht="30">
       <c r="A206" s="1" t="s">
         <v>209</v>
       </c>
@@ -6061,10 +6061,10 @@
         <v>288</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" ht="45">
       <c r="A207" s="1" t="s">
         <v>210</v>
       </c>
@@ -6078,10 +6078,10 @@
         <v>288</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" ht="60">
       <c r="A208" s="1" t="s">
         <v>211</v>
       </c>
@@ -6095,10 +6095,10 @@
         <v>288</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
       <c r="A209" s="1" t="s">
         <v>212</v>
       </c>
@@ -6112,10 +6112,10 @@
         <v>288</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" ht="60">
       <c r="A210" s="1" t="s">
         <v>213</v>
       </c>
@@ -6129,10 +6129,10 @@
         <v>288</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
       <c r="A211" s="1" t="s">
         <v>214</v>
       </c>
@@ -6146,10 +6146,10 @@
         <v>288</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" ht="30">
       <c r="A212" s="1" t="s">
         <v>215</v>
       </c>
@@ -6163,10 +6163,10 @@
         <v>288</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" ht="30">
       <c r="A213" s="1" t="s">
         <v>216</v>
       </c>
@@ -6180,10 +6180,10 @@
         <v>288</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" ht="45">
       <c r="A214" s="1" t="s">
         <v>217</v>
       </c>
@@ -6197,10 +6197,10 @@
         <v>288</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" ht="45">
       <c r="A215" s="1" t="s">
         <v>218</v>
       </c>
@@ -6214,10 +6214,10 @@
         <v>288</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" ht="30">
       <c r="A216" s="1" t="s">
         <v>219</v>
       </c>
@@ -6231,10 +6231,10 @@
         <v>288</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" ht="30">
       <c r="A217" s="1" t="s">
         <v>220</v>
       </c>
@@ -6248,10 +6248,10 @@
         <v>288</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" ht="30">
       <c r="A218" s="1" t="s">
         <v>221</v>
       </c>
@@ -6265,10 +6265,10 @@
         <v>288</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" ht="30">
       <c r="A219" s="1" t="s">
         <v>222</v>
       </c>
@@ -6282,10 +6282,10 @@
         <v>288</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" ht="45">
       <c r="A220" s="1" t="s">
         <v>223</v>
       </c>
@@ -6299,10 +6299,10 @@
         <v>288</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" ht="30">
       <c r="A221" s="1" t="s">
         <v>224</v>
       </c>
@@ -6316,10 +6316,10 @@
         <v>288</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5">
       <c r="A222" s="1" t="s">
         <v>225</v>
       </c>
@@ -6333,10 +6333,10 @@
         <v>288</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" ht="30">
       <c r="A223" s="1" t="s">
         <v>226</v>
       </c>
@@ -6350,10 +6350,10 @@
         <v>288</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5">
       <c r="A224" s="1" t="s">
         <v>227</v>
       </c>
@@ -6367,10 +6367,10 @@
         <v>288</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" ht="30">
       <c r="A225" s="1" t="s">
         <v>228</v>
       </c>
@@ -6384,10 +6384,10 @@
         <v>288</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="226" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" ht="30">
       <c r="A226" s="1" t="s">
         <v>229</v>
       </c>
@@ -6401,10 +6401,10 @@
         <v>288</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5">
       <c r="A227" s="1" t="s">
         <v>230</v>
       </c>
@@ -6418,10 +6418,10 @@
         <v>288</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5">
       <c r="A228" s="1" t="s">
         <v>231</v>
       </c>
@@ -6435,10 +6435,10 @@
         <v>288</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5">
       <c r="A229" s="1" t="s">
         <v>232</v>
       </c>
@@ -6452,10 +6452,10 @@
         <v>288</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5">
       <c r="A230" s="1" t="s">
         <v>233</v>
       </c>
@@ -6469,10 +6469,10 @@
         <v>288</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5">
       <c r="A231" s="1" t="s">
         <v>234</v>
       </c>
@@ -6486,10 +6486,10 @@
         <v>288</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5">
       <c r="A232" s="1" t="s">
         <v>235</v>
       </c>
@@ -6503,10 +6503,10 @@
         <v>288</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5">
       <c r="A233" s="1" t="s">
         <v>236</v>
       </c>
@@ -6520,10 +6520,10 @@
         <v>288</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5">
       <c r="A234" s="1" t="s">
         <v>237</v>
       </c>
@@ -6537,10 +6537,10 @@
         <v>288</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5">
       <c r="A235" s="1" t="s">
         <v>238</v>
       </c>
@@ -6554,10 +6554,10 @@
         <v>288</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5">
       <c r="A236" s="1" t="s">
         <v>239</v>
       </c>
@@ -6571,10 +6571,10 @@
         <v>288</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5">
       <c r="A237" s="1" t="s">
         <v>240</v>
       </c>
@@ -6588,10 +6588,10 @@
         <v>288</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5">
       <c r="A238" s="1" t="s">
         <v>241</v>
       </c>
@@ -6605,10 +6605,10 @@
         <v>288</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5">
       <c r="A239" s="1" t="s">
         <v>242</v>
       </c>
@@ -6622,10 +6622,10 @@
         <v>288</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5">
       <c r="A240" s="1" t="s">
         <v>243</v>
       </c>
@@ -6639,10 +6639,10 @@
         <v>288</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5">
       <c r="A241" s="1" t="s">
         <v>244</v>
       </c>
@@ -6656,10 +6656,10 @@
         <v>288</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5">
       <c r="A242" s="1" t="s">
         <v>245</v>
       </c>
@@ -6673,10 +6673,10 @@
         <v>288</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5">
       <c r="A243" s="1" t="s">
         <v>246</v>
       </c>
@@ -6690,10 +6690,10 @@
         <v>288</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5">
       <c r="A244" s="1" t="s">
         <v>247</v>
       </c>
@@ -6707,10 +6707,10 @@
         <v>288</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5">
       <c r="A245" s="1" t="s">
         <v>248</v>
       </c>
@@ -6724,10 +6724,10 @@
         <v>288</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5">
       <c r="A246" s="1" t="s">
         <v>249</v>
       </c>
@@ -6741,10 +6741,10 @@
         <v>288</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5">
       <c r="A247" s="1" t="s">
         <v>250</v>
       </c>
@@ -6758,10 +6758,10 @@
         <v>288</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="248" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" ht="75">
       <c r="A248" s="1" t="s">
         <v>251</v>
       </c>
@@ -6775,10 +6775,10 @@
         <v>288</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5">
       <c r="A249" s="1" t="s">
         <v>252</v>
       </c>
@@ -6792,10 +6792,10 @@
         <v>288</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5">
       <c r="A250" s="1" t="s">
         <v>253</v>
       </c>
@@ -6809,10 +6809,10 @@
         <v>288</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5">
       <c r="A251" s="1" t="s">
         <v>254</v>
       </c>
@@ -6826,10 +6826,10 @@
         <v>288</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5">
       <c r="A252" s="1" t="s">
         <v>255</v>
       </c>
@@ -6843,10 +6843,10 @@
         <v>288</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5">
       <c r="A253" s="1" t="s">
         <v>256</v>
       </c>
@@ -6860,10 +6860,10 @@
         <v>288</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5">
       <c r="A254" s="1" t="s">
         <v>238</v>
       </c>
@@ -6877,10 +6877,10 @@
         <v>288</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" ht="30">
       <c r="A255" s="1" t="s">
         <v>257</v>
       </c>
@@ -6894,10 +6894,10 @@
         <v>288</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5">
       <c r="A256" s="1" t="s">
         <v>258</v>
       </c>
@@ -6911,10 +6911,10 @@
         <v>288</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5">
       <c r="A257" s="1" t="s">
         <v>259</v>
       </c>
@@ -6928,10 +6928,10 @@
         <v>288</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5">
       <c r="A258" s="1" t="s">
         <v>260</v>
       </c>
@@ -6945,10 +6945,10 @@
         <v>288</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5">
       <c r="A259" s="1" t="s">
         <v>261</v>
       </c>
@@ -6962,10 +6962,10 @@
         <v>288</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="260" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" ht="30">
       <c r="A260" s="1" t="s">
         <v>262</v>
       </c>
@@ -6979,10 +6979,10 @@
         <v>288</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5">
       <c r="A261" s="1" t="s">
         <v>263</v>
       </c>
@@ -6996,10 +6996,10 @@
         <v>288</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="262" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" ht="30">
       <c r="A262" s="1" t="s">
         <v>264</v>
       </c>
@@ -7013,10 +7013,10 @@
         <v>288</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="263" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" ht="30">
       <c r="A263" s="1" t="s">
         <v>265</v>
       </c>
@@ -7030,10 +7030,10 @@
         <v>288</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="264" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" ht="45">
       <c r="A264" s="1" t="s">
         <v>266</v>
       </c>
@@ -7047,10 +7047,10 @@
         <v>288</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="265" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" ht="30">
       <c r="A265" s="1" t="s">
         <v>267</v>
       </c>
@@ -7064,10 +7064,10 @@
         <v>288</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="266" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" ht="45">
       <c r="A266" s="1" t="s">
         <v>268</v>
       </c>
@@ -7081,10 +7081,10 @@
         <v>288</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="267" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5">
       <c r="A267" s="1" t="s">
         <v>269</v>
       </c>
@@ -7098,10 +7098,10 @@
         <v>288</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="268" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" ht="45">
       <c r="A268" s="1" t="s">
         <v>270</v>
       </c>
@@ -7115,10 +7115,10 @@
         <v>288</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="269" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" ht="45">
       <c r="A269" s="1" t="s">
         <v>271</v>
       </c>
@@ -7132,10 +7132,10 @@
         <v>288</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="270" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" ht="60">
       <c r="A270" s="1" t="s">
         <v>272</v>
       </c>
@@ -7149,10 +7149,10 @@
         <v>288</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="271" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" ht="30">
       <c r="A271" s="1" t="s">
         <v>273</v>
       </c>
@@ -7166,10 +7166,10 @@
         <v>288</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="272" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" ht="60">
       <c r="A272" s="1" t="s">
         <v>274</v>
       </c>
@@ -7183,10 +7183,10 @@
         <v>288</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="273" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" ht="45">
       <c r="A273" s="1" t="s">
         <v>275</v>
       </c>
@@ -7200,10 +7200,10 @@
         <v>288</v>
       </c>
       <c r="E273" s="1" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="274" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" ht="45">
       <c r="A274" s="1" t="s">
         <v>276</v>
       </c>
@@ -7217,10 +7217,10 @@
         <v>288</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="275" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" ht="45">
       <c r="A275" s="1" t="s">
         <v>277</v>
       </c>
@@ -7234,10 +7234,10 @@
         <v>288</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="276" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" ht="30">
       <c r="A276" s="1" t="s">
         <v>278</v>
       </c>
@@ -7251,10 +7251,10 @@
         <v>288</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="277" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" ht="30">
       <c r="A277" s="1" t="s">
         <v>279</v>
       </c>
@@ -7268,10 +7268,10 @@
         <v>288</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="278" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" ht="30">
       <c r="A278" s="1" t="s">
         <v>280</v>
       </c>
@@ -7285,10 +7285,10 @@
         <v>288</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="279" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" ht="30">
       <c r="A279" s="1" t="s">
         <v>281</v>
       </c>
@@ -7302,10 +7302,10 @@
         <v>288</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="280" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5">
       <c r="A280" s="1" t="s">
         <v>282</v>
       </c>
@@ -7319,7 +7319,7 @@
         <v>288</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
   </sheetData>
@@ -7331,24 +7331,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Header corrections. Brand new printf() implementation. OS debug and debug partly re-written. Changes to os_config interface to better reflect BSW generator. Arm Cortex cleanup. Arm not Tested. PPC runs testsystem OK on T32.
</commit_message>
<xml_diff>
--- a/scripts/req-os.xlsx
+++ b/scripts/req-os.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="465" windowWidth="27555" windowHeight="14025"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="609">
   <si>
     <t>id</t>
   </si>
@@ -2129,6 +2129,110 @@
   </si>
   <si>
     <t>1,2</t>
+  </si>
+  <si>
+    <t>OSEK001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interrupts have precedence over tasks </t>
+  </si>
+  <si>
+    <t>OSEK002</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The interrupt processing level consists of one or more interrupt priority levels </t>
+  </si>
+  <si>
+    <t>OSEK003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interrupt service routines have a statically assigned interrupt priority level </t>
+  </si>
+  <si>
+    <t>OSEK004</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Assignment of interrupt service routines to interrupt priority levels is dependent on implementation and hardware architecture </t>
+  </si>
+  <si>
+    <t>OSEK005</t>
+  </si>
+  <si>
+    <t>OSEK006</t>
+  </si>
+  <si>
+    <t>The task’s priority is statically assigned by the user</t>
+  </si>
+  <si>
+    <t>OSEK007</t>
+  </si>
+  <si>
+    <t>Basic Tasks must support multiple activation</t>
+  </si>
+  <si>
+    <t>OSEK008</t>
+  </si>
+  <si>
+    <t>Extended tasks is limited to one activation.</t>
+  </si>
+  <si>
+    <t>OSEK009</t>
+  </si>
+  <si>
+    <t>Basic tasks release the processor if, they terminate, the OS swiches to higher priotiry task or an interrupt occurs which causes the processor to switch to an interrupt service routine.</t>
+  </si>
+  <si>
+    <t>OSEK010</t>
+  </si>
+  <si>
+    <t>Extended task have the following states: running, ready, waiting and suspended.</t>
+  </si>
+  <si>
+    <t>OSEK011</t>
+  </si>
+  <si>
+    <t>Basic tasks have the following states: running, ready and suspended</t>
+  </si>
+  <si>
+    <t>OSEK012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Multiple requesting of task activation" means that the OSEK operating system receives and records parallel activations of a basic task already activated. The number of multiple requests in parallel is defined in a basic task specific attribute during 
+system  generation.  If  the  maximum  number  of  multiple  requests  has  not  been  reached,  the request is queued. The requests of basic task activations are queued per priority in activation order. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For task priorities and resource ceiling-priorities bigger numbers refer to higher priorities. The  value  0  is  defined  as  the  lowest  priority  of  a  task.  Accordingly  bigger  numbers  define higher priorities. </t>
+  </si>
+  <si>
+    <t>OSEK013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasks on the same priority level are started depending on their order of activation, extended  tasks  in  the  waiting  state  do  not  block  the  start  of  subsequent  tasks  of  identical priority. whereby </t>
+  </si>
+  <si>
+    <t>OSEK014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A  preempted  task  is  considered  to  be  the  first  (oldest)  task  in  the  ready  list  of  its  current priority. </t>
+  </si>
+  <si>
+    <t>OSEK015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A task being released from the waiting state is treated like the last (newest) task in the ready queue of its priority. </t>
+  </si>
+  <si>
+    <t>OSEK016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The following fundamental steps are necessary to determine the next task to be processed: 1.  The scheduler searches for all tasks in the ready/running state. 2.  From the set of tasks in the ready/running state, the scheduler determines the set of 
+tasks with the highest priority. 3.  Within the set of tasks in the ready/running state and of highest priority, the scheduler finds the oldest task. </t>
+  </si>
+  <si>
+    <t>OSEK17</t>
   </si>
 </sst>
 </file>
@@ -2164,12 +2268,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2238,8 +2345,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E280" tableType="xml" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" connectionId="1">
-  <autoFilter ref="A1:E280"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E297" tableType="xml" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" connectionId="1">
+  <autoFilter ref="A1:E297">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="code,generator"/>
+        <filter val="generator"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="5">
     <tableColumn id="1" uniqueName="id" name="id" dataDxfId="4">
       <xmlColumnPr mapId="1" xpath="/ns1:Requirements/ns1:Req/@id" xmlDataType="string"/>
@@ -2546,15 +2660,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E280"/>
+  <dimension ref="A1:E297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="E278" sqref="E278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" style="2" customWidth="1"/>
@@ -2579,7 +2693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30">
+    <row r="2" spans="1:5" ht="30" hidden="1">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2596,7 +2710,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" hidden="1">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2613,7 +2727,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30">
+    <row r="4" spans="1:5" ht="30" hidden="1">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2630,7 +2744,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30">
+    <row r="5" spans="1:5" ht="30" hidden="1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2647,7 +2761,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30">
+    <row r="6" spans="1:5" ht="30" hidden="1">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2664,7 +2778,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" hidden="1">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2681,7 +2795,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:5" ht="30" hidden="1">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -2698,7 +2812,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" hidden="1">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -2715,7 +2829,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30">
+    <row r="10" spans="1:5" ht="30" hidden="1">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -2732,7 +2846,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="60">
+    <row r="11" spans="1:5" ht="60" hidden="1">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -2749,7 +2863,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="30" hidden="1">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -2766,7 +2880,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="45">
+    <row r="13" spans="1:5" ht="45" hidden="1">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -2936,7 +3050,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="45">
+    <row r="23" spans="1:5" ht="45" hidden="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -2953,7 +3067,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" hidden="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -2970,7 +3084,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" hidden="1">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -2987,7 +3101,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30">
+    <row r="26" spans="1:5" ht="30" hidden="1">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -3004,7 +3118,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" hidden="1">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -3021,7 +3135,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30">
+    <row r="28" spans="1:5" ht="30" hidden="1">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -3055,7 +3169,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="45">
+    <row r="30" spans="1:5" ht="45" hidden="1">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -3072,7 +3186,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" hidden="1">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -3089,7 +3203,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="45">
+    <row r="32" spans="1:5" ht="45" hidden="1">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -3106,7 +3220,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" hidden="1">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -3123,7 +3237,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" hidden="1">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -3140,7 +3254,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" hidden="1">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -3157,7 +3271,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="45">
+    <row r="36" spans="1:5" ht="45" hidden="1">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -3174,7 +3288,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="30">
+    <row r="37" spans="1:5" ht="30" hidden="1">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -3191,7 +3305,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" hidden="1">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -3208,7 +3322,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30">
+    <row r="39" spans="1:5" ht="30" hidden="1">
       <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
@@ -3225,7 +3339,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="30">
+    <row r="40" spans="1:5" ht="30" hidden="1">
       <c r="A40" s="1" t="s">
         <v>43</v>
       </c>
@@ -3242,7 +3356,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" hidden="1">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -3259,7 +3373,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="30">
+    <row r="42" spans="1:5" ht="30" hidden="1">
       <c r="A42" s="1" t="s">
         <v>45</v>
       </c>
@@ -3276,7 +3390,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="30">
+    <row r="43" spans="1:5" ht="30" hidden="1">
       <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
@@ -3293,7 +3407,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="30">
+    <row r="44" spans="1:5" ht="30" hidden="1">
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
@@ -3310,7 +3424,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="45">
+    <row r="45" spans="1:5" ht="45" hidden="1">
       <c r="A45" s="1" t="s">
         <v>48</v>
       </c>
@@ -3327,7 +3441,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="30">
+    <row r="46" spans="1:5" ht="30" hidden="1">
       <c r="A46" s="1" t="s">
         <v>49</v>
       </c>
@@ -3344,7 +3458,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" hidden="1">
       <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
@@ -3361,7 +3475,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" hidden="1">
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
@@ -3378,7 +3492,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" hidden="1">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -3395,7 +3509,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="45">
+    <row r="50" spans="1:5" ht="45" hidden="1">
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
@@ -3412,7 +3526,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="45">
+    <row r="51" spans="1:5" ht="45" hidden="1">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
@@ -3429,7 +3543,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="30">
+    <row r="52" spans="1:5" ht="30" hidden="1">
       <c r="A52" s="1" t="s">
         <v>55</v>
       </c>
@@ -3446,7 +3560,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="30">
+    <row r="53" spans="1:5" ht="30" hidden="1">
       <c r="A53" s="1" t="s">
         <v>56</v>
       </c>
@@ -3463,7 +3577,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="30">
+    <row r="54" spans="1:5" ht="30" hidden="1">
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
@@ -3480,7 +3594,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="45">
+    <row r="55" spans="1:5" ht="45" hidden="1">
       <c r="A55" s="1" t="s">
         <v>58</v>
       </c>
@@ -3497,7 +3611,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="30">
+    <row r="56" spans="1:5" ht="30" hidden="1">
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
@@ -3514,7 +3628,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" hidden="1">
       <c r="A57" s="1" t="s">
         <v>60</v>
       </c>
@@ -3531,7 +3645,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" hidden="1">
       <c r="A58" s="1" t="s">
         <v>61</v>
       </c>
@@ -3548,7 +3662,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="45">
+    <row r="59" spans="1:5" ht="45" hidden="1">
       <c r="A59" s="1" t="s">
         <v>62</v>
       </c>
@@ -3565,7 +3679,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" hidden="1">
       <c r="A60" s="1" t="s">
         <v>63</v>
       </c>
@@ -3582,7 +3696,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="30">
+    <row r="61" spans="1:5" ht="30" hidden="1">
       <c r="A61" s="1" t="s">
         <v>64</v>
       </c>
@@ -3599,7 +3713,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="30">
+    <row r="62" spans="1:5" ht="30" hidden="1">
       <c r="A62" s="1" t="s">
         <v>65</v>
       </c>
@@ -3633,7 +3747,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="45">
+    <row r="64" spans="1:5" ht="45" hidden="1">
       <c r="A64" s="1" t="s">
         <v>67</v>
       </c>
@@ -3650,7 +3764,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="45">
+    <row r="65" spans="1:5" ht="45" hidden="1">
       <c r="A65" s="1" t="s">
         <v>68</v>
       </c>
@@ -3667,7 +3781,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="60">
+    <row r="66" spans="1:5" ht="60" hidden="1">
       <c r="A66" s="1" t="s">
         <v>69</v>
       </c>
@@ -3684,7 +3798,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="30">
+    <row r="67" spans="1:5" ht="30" hidden="1">
       <c r="A67" s="1" t="s">
         <v>70</v>
       </c>
@@ -3701,7 +3815,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="30">
+    <row r="68" spans="1:5" ht="30" hidden="1">
       <c r="A68" s="1" t="s">
         <v>71</v>
       </c>
@@ -3718,7 +3832,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="30">
+    <row r="69" spans="1:5" ht="30" hidden="1">
       <c r="A69" s="1" t="s">
         <v>72</v>
       </c>
@@ -3735,7 +3849,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="45">
+    <row r="70" spans="1:5" ht="45" hidden="1">
       <c r="A70" s="1" t="s">
         <v>73</v>
       </c>
@@ -3752,7 +3866,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="45">
+    <row r="71" spans="1:5" ht="45" hidden="1">
       <c r="A71" s="1" t="s">
         <v>74</v>
       </c>
@@ -3769,7 +3883,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="60">
+    <row r="72" spans="1:5" ht="60" hidden="1">
       <c r="A72" s="1" t="s">
         <v>75</v>
       </c>
@@ -3786,7 +3900,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" hidden="1">
       <c r="A73" s="1" t="s">
         <v>76</v>
       </c>
@@ -3803,7 +3917,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="45">
+    <row r="74" spans="1:5" ht="45" hidden="1">
       <c r="A74" s="1" t="s">
         <v>77</v>
       </c>
@@ -3820,7 +3934,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" hidden="1">
       <c r="A75" s="1" t="s">
         <v>78</v>
       </c>
@@ -3837,7 +3951,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="30">
+    <row r="76" spans="1:5" ht="30" hidden="1">
       <c r="A76" s="1" t="s">
         <v>79</v>
       </c>
@@ -3854,7 +3968,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="30">
+    <row r="77" spans="1:5" ht="30" hidden="1">
       <c r="A77" s="1" t="s">
         <v>80</v>
       </c>
@@ -3871,7 +3985,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="30">
+    <row r="78" spans="1:5" ht="30" hidden="1">
       <c r="A78" s="1" t="s">
         <v>81</v>
       </c>
@@ -3888,7 +4002,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="30">
+    <row r="79" spans="1:5" ht="30" hidden="1">
       <c r="A79" s="1" t="s">
         <v>82</v>
       </c>
@@ -3905,7 +4019,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="45">
+    <row r="80" spans="1:5" ht="45" hidden="1">
       <c r="A80" s="1" t="s">
         <v>83</v>
       </c>
@@ -3922,7 +4036,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="45">
+    <row r="81" spans="1:5" ht="45" hidden="1">
       <c r="A81" s="1" t="s">
         <v>84</v>
       </c>
@@ -3939,7 +4053,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" hidden="1">
       <c r="A82" s="1" t="s">
         <v>85</v>
       </c>
@@ -3956,7 +4070,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="45">
+    <row r="83" spans="1:5" ht="45" hidden="1">
       <c r="A83" s="1" t="s">
         <v>86</v>
       </c>
@@ -3973,7 +4087,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="45">
+    <row r="84" spans="1:5" ht="45" hidden="1">
       <c r="A84" s="1" t="s">
         <v>87</v>
       </c>
@@ -3990,7 +4104,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="30">
+    <row r="85" spans="1:5" ht="30" hidden="1">
       <c r="A85" s="1" t="s">
         <v>88</v>
       </c>
@@ -4007,7 +4121,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="30">
+    <row r="86" spans="1:5" ht="30" hidden="1">
       <c r="A86" s="1" t="s">
         <v>89</v>
       </c>
@@ -4024,7 +4138,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="30">
+    <row r="87" spans="1:5" ht="30" hidden="1">
       <c r="A87" s="1" t="s">
         <v>90</v>
       </c>
@@ -4041,7 +4155,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="45">
+    <row r="88" spans="1:5" ht="45" hidden="1">
       <c r="A88" s="1" t="s">
         <v>91</v>
       </c>
@@ -4058,7 +4172,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="30">
+    <row r="89" spans="1:5" ht="30" hidden="1">
       <c r="A89" s="1" t="s">
         <v>92</v>
       </c>
@@ -4075,7 +4189,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="30">
+    <row r="90" spans="1:5" ht="30" hidden="1">
       <c r="A90" s="1" t="s">
         <v>93</v>
       </c>
@@ -4092,7 +4206,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="30">
+    <row r="91" spans="1:5" ht="30" hidden="1">
       <c r="A91" s="1" t="s">
         <v>94</v>
       </c>
@@ -4109,7 +4223,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="30">
+    <row r="92" spans="1:5" ht="30" hidden="1">
       <c r="A92" s="1" t="s">
         <v>95</v>
       </c>
@@ -4126,7 +4240,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="30">
+    <row r="93" spans="1:5" ht="30" hidden="1">
       <c r="A93" s="1" t="s">
         <v>96</v>
       </c>
@@ -4143,7 +4257,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="30">
+    <row r="94" spans="1:5" ht="30" hidden="1">
       <c r="A94" s="1" t="s">
         <v>97</v>
       </c>
@@ -4160,7 +4274,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="30">
+    <row r="95" spans="1:5" ht="30" hidden="1">
       <c r="A95" s="1" t="s">
         <v>98</v>
       </c>
@@ -4177,7 +4291,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="30">
+    <row r="96" spans="1:5" ht="30" hidden="1">
       <c r="A96" s="1" t="s">
         <v>99</v>
       </c>
@@ -4194,7 +4308,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="30">
+    <row r="97" spans="1:5" ht="30" hidden="1">
       <c r="A97" s="1" t="s">
         <v>100</v>
       </c>
@@ -4211,7 +4325,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="45">
+    <row r="98" spans="1:5" ht="45" hidden="1">
       <c r="A98" s="1" t="s">
         <v>101</v>
       </c>
@@ -4228,7 +4342,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="45">
+    <row r="99" spans="1:5" ht="45" hidden="1">
       <c r="A99" s="1" t="s">
         <v>102</v>
       </c>
@@ -4245,7 +4359,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="30">
+    <row r="100" spans="1:5" ht="30" hidden="1">
       <c r="A100" s="1" t="s">
         <v>103</v>
       </c>
@@ -4262,7 +4376,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" hidden="1">
       <c r="A101" s="1" t="s">
         <v>104</v>
       </c>
@@ -4279,7 +4393,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="30">
+    <row r="102" spans="1:5" ht="30" hidden="1">
       <c r="A102" s="1" t="s">
         <v>105</v>
       </c>
@@ -4296,7 +4410,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="60">
+    <row r="103" spans="1:5" ht="60" hidden="1">
       <c r="A103" s="1" t="s">
         <v>106</v>
       </c>
@@ -4313,7 +4427,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="45">
+    <row r="104" spans="1:5" ht="45" hidden="1">
       <c r="A104" s="1" t="s">
         <v>107</v>
       </c>
@@ -4330,7 +4444,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="45">
+    <row r="105" spans="1:5" ht="45" hidden="1">
       <c r="A105" s="1" t="s">
         <v>108</v>
       </c>
@@ -4347,7 +4461,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="60">
+    <row r="106" spans="1:5" ht="60" hidden="1">
       <c r="A106" s="1" t="s">
         <v>109</v>
       </c>
@@ -4364,7 +4478,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="45">
+    <row r="107" spans="1:5" ht="45" hidden="1">
       <c r="A107" s="1" t="s">
         <v>110</v>
       </c>
@@ -4381,7 +4495,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" hidden="1">
       <c r="A108" s="1" t="s">
         <v>111</v>
       </c>
@@ -4398,7 +4512,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="45">
+    <row r="109" spans="1:5" ht="45" hidden="1">
       <c r="A109" s="1" t="s">
         <v>112</v>
       </c>
@@ -4415,7 +4529,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" hidden="1">
       <c r="A110" s="1" t="s">
         <v>113</v>
       </c>
@@ -4432,7 +4546,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="45">
+    <row r="111" spans="1:5" ht="45" hidden="1">
       <c r="A111" s="1" t="s">
         <v>114</v>
       </c>
@@ -4449,7 +4563,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="45">
+    <row r="112" spans="1:5" ht="45" hidden="1">
       <c r="A112" s="1" t="s">
         <v>115</v>
       </c>
@@ -4466,7 +4580,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" hidden="1">
       <c r="A113" s="1" t="s">
         <v>116</v>
       </c>
@@ -4483,7 +4597,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="60">
+    <row r="114" spans="1:5" ht="60" hidden="1">
       <c r="A114" s="1" t="s">
         <v>117</v>
       </c>
@@ -4500,7 +4614,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="30">
+    <row r="115" spans="1:5" ht="30" hidden="1">
       <c r="A115" s="1" t="s">
         <v>118</v>
       </c>
@@ -4517,7 +4631,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="60">
+    <row r="116" spans="1:5" ht="60" hidden="1">
       <c r="A116" s="1" t="s">
         <v>119</v>
       </c>
@@ -4534,7 +4648,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" hidden="1">
       <c r="A117" s="1" t="s">
         <v>120</v>
       </c>
@@ -4551,7 +4665,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="30">
+    <row r="118" spans="1:5" ht="30" hidden="1">
       <c r="A118" s="1" t="s">
         <v>121</v>
       </c>
@@ -4568,7 +4682,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" hidden="1">
       <c r="A119" s="1" t="s">
         <v>122</v>
       </c>
@@ -4585,7 +4699,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="45">
+    <row r="120" spans="1:5" ht="45" hidden="1">
       <c r="A120" s="1" t="s">
         <v>123</v>
       </c>
@@ -4602,7 +4716,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="45">
+    <row r="121" spans="1:5" ht="45" hidden="1">
       <c r="A121" s="1" t="s">
         <v>124</v>
       </c>
@@ -4619,7 +4733,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="30">
+    <row r="122" spans="1:5" ht="30" hidden="1">
       <c r="A122" s="1" t="s">
         <v>125</v>
       </c>
@@ -4636,7 +4750,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="45">
+    <row r="123" spans="1:5" ht="45" hidden="1">
       <c r="A123" s="1" t="s">
         <v>126</v>
       </c>
@@ -4653,7 +4767,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="30">
+    <row r="124" spans="1:5" ht="30" hidden="1">
       <c r="A124" s="1" t="s">
         <v>127</v>
       </c>
@@ -4670,7 +4784,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="30">
+    <row r="125" spans="1:5" ht="30" hidden="1">
       <c r="A125" s="1" t="s">
         <v>128</v>
       </c>
@@ -4687,7 +4801,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="30">
+    <row r="126" spans="1:5" ht="30" hidden="1">
       <c r="A126" s="1" t="s">
         <v>129</v>
       </c>
@@ -4704,7 +4818,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="30">
+    <row r="127" spans="1:5" ht="30" hidden="1">
       <c r="A127" s="1" t="s">
         <v>130</v>
       </c>
@@ -4721,7 +4835,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="45">
+    <row r="128" spans="1:5" ht="45" hidden="1">
       <c r="A128" s="1" t="s">
         <v>131</v>
       </c>
@@ -4738,7 +4852,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="30">
+    <row r="129" spans="1:5" ht="30" hidden="1">
       <c r="A129" s="1" t="s">
         <v>132</v>
       </c>
@@ -4755,7 +4869,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" hidden="1">
       <c r="A130" s="1" t="s">
         <v>133</v>
       </c>
@@ -4772,7 +4886,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="30">
+    <row r="131" spans="1:5" ht="30" hidden="1">
       <c r="A131" s="1" t="s">
         <v>134</v>
       </c>
@@ -4789,7 +4903,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="30">
+    <row r="132" spans="1:5" ht="30" hidden="1">
       <c r="A132" s="1" t="s">
         <v>135</v>
       </c>
@@ -4806,7 +4920,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="45">
+    <row r="133" spans="1:5" ht="45" hidden="1">
       <c r="A133" s="1" t="s">
         <v>136</v>
       </c>
@@ -4823,7 +4937,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="30">
+    <row r="134" spans="1:5" ht="30" hidden="1">
       <c r="A134" s="1" t="s">
         <v>137</v>
       </c>
@@ -4840,7 +4954,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:5" hidden="1">
       <c r="A135" s="1" t="s">
         <v>138</v>
       </c>
@@ -4857,7 +4971,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" hidden="1">
       <c r="A136" s="1" t="s">
         <v>139</v>
       </c>
@@ -4874,7 +4988,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" hidden="1">
       <c r="A137" s="1" t="s">
         <v>140</v>
       </c>
@@ -4891,7 +5005,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="30">
+    <row r="138" spans="1:5" ht="30" hidden="1">
       <c r="A138" s="1" t="s">
         <v>141</v>
       </c>
@@ -4908,7 +5022,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="30">
+    <row r="139" spans="1:5" ht="30" hidden="1">
       <c r="A139" s="1" t="s">
         <v>142</v>
       </c>
@@ -4925,7 +5039,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="30">
+    <row r="140" spans="1:5" ht="30" hidden="1">
       <c r="A140" s="1" t="s">
         <v>143</v>
       </c>
@@ -4942,7 +5056,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="30">
+    <row r="141" spans="1:5" ht="30" hidden="1">
       <c r="A141" s="1" t="s">
         <v>144</v>
       </c>
@@ -4959,7 +5073,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="45">
+    <row r="142" spans="1:5" ht="45" hidden="1">
       <c r="A142" s="1" t="s">
         <v>145</v>
       </c>
@@ -4976,7 +5090,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="30">
+    <row r="143" spans="1:5" ht="30" hidden="1">
       <c r="A143" s="1" t="s">
         <v>146</v>
       </c>
@@ -4993,7 +5107,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="30">
+    <row r="144" spans="1:5" ht="30" hidden="1">
       <c r="A144" s="1" t="s">
         <v>147</v>
       </c>
@@ -5010,7 +5124,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="45">
+    <row r="145" spans="1:5" ht="45" hidden="1">
       <c r="A145" s="1" t="s">
         <v>148</v>
       </c>
@@ -5027,7 +5141,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="45">
+    <row r="146" spans="1:5" ht="45" hidden="1">
       <c r="A146" s="1" t="s">
         <v>149</v>
       </c>
@@ -5044,7 +5158,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="30">
+    <row r="147" spans="1:5" ht="30" hidden="1">
       <c r="A147" s="1" t="s">
         <v>150</v>
       </c>
@@ -5061,7 +5175,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="60">
+    <row r="148" spans="1:5" ht="60" hidden="1">
       <c r="A148" s="1" t="s">
         <v>151</v>
       </c>
@@ -5078,7 +5192,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" hidden="1">
       <c r="A149" s="1" t="s">
         <v>152</v>
       </c>
@@ -5095,7 +5209,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="30">
+    <row r="150" spans="1:5" ht="30" hidden="1">
       <c r="A150" s="1" t="s">
         <v>153</v>
       </c>
@@ -5112,7 +5226,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="30">
+    <row r="151" spans="1:5" ht="30" hidden="1">
       <c r="A151" s="1" t="s">
         <v>154</v>
       </c>
@@ -5129,7 +5243,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="30">
+    <row r="152" spans="1:5" ht="30" hidden="1">
       <c r="A152" s="1" t="s">
         <v>155</v>
       </c>
@@ -5146,7 +5260,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="30">
+    <row r="153" spans="1:5" ht="30" hidden="1">
       <c r="A153" s="1" t="s">
         <v>156</v>
       </c>
@@ -5163,7 +5277,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="30">
+    <row r="154" spans="1:5" ht="30" hidden="1">
       <c r="A154" s="1" t="s">
         <v>157</v>
       </c>
@@ -5180,7 +5294,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="45">
+    <row r="155" spans="1:5" ht="45" hidden="1">
       <c r="A155" s="1" t="s">
         <v>158</v>
       </c>
@@ -5197,7 +5311,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" hidden="1">
       <c r="A156" s="1" t="s">
         <v>159</v>
       </c>
@@ -5214,7 +5328,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="60">
+    <row r="157" spans="1:5" ht="60" hidden="1">
       <c r="A157" s="1" t="s">
         <v>160</v>
       </c>
@@ -5231,7 +5345,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="30">
+    <row r="158" spans="1:5" ht="30" hidden="1">
       <c r="A158" s="1" t="s">
         <v>161</v>
       </c>
@@ -5248,7 +5362,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="45">
+    <row r="159" spans="1:5" ht="45" hidden="1">
       <c r="A159" s="1" t="s">
         <v>162</v>
       </c>
@@ -5265,7 +5379,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="45">
+    <row r="160" spans="1:5" ht="45" hidden="1">
       <c r="A160" s="1" t="s">
         <v>163</v>
       </c>
@@ -5282,7 +5396,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="30">
+    <row r="161" spans="1:5" ht="30" hidden="1">
       <c r="A161" s="1" t="s">
         <v>164</v>
       </c>
@@ -5299,7 +5413,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="30">
+    <row r="162" spans="1:5" ht="30" hidden="1">
       <c r="A162" s="1" t="s">
         <v>165</v>
       </c>
@@ -5316,7 +5430,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="30">
+    <row r="163" spans="1:5" ht="30" hidden="1">
       <c r="A163" s="1" t="s">
         <v>166</v>
       </c>
@@ -5333,7 +5447,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="30">
+    <row r="164" spans="1:5" ht="30" hidden="1">
       <c r="A164" s="1" t="s">
         <v>167</v>
       </c>
@@ -5350,7 +5464,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="30">
+    <row r="165" spans="1:5" ht="30" hidden="1">
       <c r="A165" s="1" t="s">
         <v>168</v>
       </c>
@@ -5367,7 +5481,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="30">
+    <row r="166" spans="1:5" ht="30" hidden="1">
       <c r="A166" s="1" t="s">
         <v>169</v>
       </c>
@@ -5384,7 +5498,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="30">
+    <row r="167" spans="1:5" ht="30" hidden="1">
       <c r="A167" s="1" t="s">
         <v>170</v>
       </c>
@@ -5401,7 +5515,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="168" spans="1:5" ht="30">
+    <row r="168" spans="1:5" ht="30" hidden="1">
       <c r="A168" s="1" t="s">
         <v>171</v>
       </c>
@@ -5418,7 +5532,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="169" spans="1:5" ht="30">
+    <row r="169" spans="1:5" ht="30" hidden="1">
       <c r="A169" s="1" t="s">
         <v>172</v>
       </c>
@@ -5435,7 +5549,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="170" spans="1:5" ht="45">
+    <row r="170" spans="1:5" ht="45" hidden="1">
       <c r="A170" s="1" t="s">
         <v>173</v>
       </c>
@@ -5452,7 +5566,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="30">
+    <row r="171" spans="1:5" ht="30" hidden="1">
       <c r="A171" s="1" t="s">
         <v>174</v>
       </c>
@@ -5469,7 +5583,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="30">
+    <row r="172" spans="1:5" ht="30" hidden="1">
       <c r="A172" s="1" t="s">
         <v>175</v>
       </c>
@@ -5486,7 +5600,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="45">
+    <row r="173" spans="1:5" ht="45" hidden="1">
       <c r="A173" s="1" t="s">
         <v>176</v>
       </c>
@@ -5503,7 +5617,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="30">
+    <row r="174" spans="1:5" ht="30" hidden="1">
       <c r="A174" s="1" t="s">
         <v>177</v>
       </c>
@@ -5520,7 +5634,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="175" spans="1:5" ht="30">
+    <row r="175" spans="1:5" ht="30" hidden="1">
       <c r="A175" s="1" t="s">
         <v>178</v>
       </c>
@@ -5537,7 +5651,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="176" spans="1:5" ht="45">
+    <row r="176" spans="1:5" ht="45" hidden="1">
       <c r="A176" s="1" t="s">
         <v>179</v>
       </c>
@@ -5554,7 +5668,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="177" spans="1:5" ht="30">
+    <row r="177" spans="1:5" ht="30" hidden="1">
       <c r="A177" s="1" t="s">
         <v>180</v>
       </c>
@@ -5571,7 +5685,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="45">
+    <row r="178" spans="1:5" ht="45" hidden="1">
       <c r="A178" s="1" t="s">
         <v>181</v>
       </c>
@@ -5588,7 +5702,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="179" spans="1:5" ht="45">
+    <row r="179" spans="1:5" ht="45" hidden="1">
       <c r="A179" s="1" t="s">
         <v>182</v>
       </c>
@@ -5605,7 +5719,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
+    <row r="180" spans="1:5" hidden="1">
       <c r="A180" s="1" t="s">
         <v>183</v>
       </c>
@@ -5622,7 +5736,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="181" spans="1:5" ht="30">
+    <row r="181" spans="1:5" ht="30" hidden="1">
       <c r="A181" s="1" t="s">
         <v>184</v>
       </c>
@@ -5639,7 +5753,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="182" spans="1:5" ht="30">
+    <row r="182" spans="1:5" ht="30" hidden="1">
       <c r="A182" s="1" t="s">
         <v>185</v>
       </c>
@@ -5656,7 +5770,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="183" spans="1:5" ht="45">
+    <row r="183" spans="1:5" ht="45" hidden="1">
       <c r="A183" s="1" t="s">
         <v>186</v>
       </c>
@@ -5673,7 +5787,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
+    <row r="184" spans="1:5" hidden="1">
       <c r="A184" s="1" t="s">
         <v>187</v>
       </c>
@@ -5690,7 +5804,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="185" spans="1:5" ht="30">
+    <row r="185" spans="1:5" ht="30" hidden="1">
       <c r="A185" s="1" t="s">
         <v>188</v>
       </c>
@@ -5707,7 +5821,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="186" spans="1:5" ht="45">
+    <row r="186" spans="1:5" ht="45" hidden="1">
       <c r="A186" s="1" t="s">
         <v>189</v>
       </c>
@@ -5724,7 +5838,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="187" spans="1:5" ht="60">
+    <row r="187" spans="1:5" ht="60" hidden="1">
       <c r="A187" s="1" t="s">
         <v>190</v>
       </c>
@@ -5741,7 +5855,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="188" spans="1:5" ht="45">
+    <row r="188" spans="1:5" ht="45" hidden="1">
       <c r="A188" s="1" t="s">
         <v>191</v>
       </c>
@@ -5758,7 +5872,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="189" spans="1:5" ht="45">
+    <row r="189" spans="1:5" ht="45" hidden="1">
       <c r="A189" s="1" t="s">
         <v>192</v>
       </c>
@@ -5775,7 +5889,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="190" spans="1:5" ht="60">
+    <row r="190" spans="1:5" ht="60" hidden="1">
       <c r="A190" s="1" t="s">
         <v>193</v>
       </c>
@@ -5792,7 +5906,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="191" spans="1:5" ht="60">
+    <row r="191" spans="1:5" ht="60" hidden="1">
       <c r="A191" s="1" t="s">
         <v>194</v>
       </c>
@@ -5809,7 +5923,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="192" spans="1:5">
+    <row r="192" spans="1:5" hidden="1">
       <c r="A192" s="1" t="s">
         <v>195</v>
       </c>
@@ -5826,7 +5940,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="75">
+    <row r="193" spans="1:5" ht="75" hidden="1">
       <c r="A193" s="1" t="s">
         <v>196</v>
       </c>
@@ -5843,7 +5957,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="194" spans="1:5" ht="45">
+    <row r="194" spans="1:5" ht="45" hidden="1">
       <c r="A194" s="1" t="s">
         <v>197</v>
       </c>
@@ -5860,7 +5974,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="195" spans="1:5" ht="30">
+    <row r="195" spans="1:5" ht="30" hidden="1">
       <c r="A195" s="1" t="s">
         <v>198</v>
       </c>
@@ -5877,7 +5991,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="196" spans="1:5" ht="60">
+    <row r="196" spans="1:5" ht="60" hidden="1">
       <c r="A196" s="1" t="s">
         <v>199</v>
       </c>
@@ -5894,7 +6008,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="197" spans="1:5" ht="30">
+    <row r="197" spans="1:5" ht="30" hidden="1">
       <c r="A197" s="1" t="s">
         <v>200</v>
       </c>
@@ -5911,7 +6025,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
+    <row r="198" spans="1:5" hidden="1">
       <c r="A198" s="1" t="s">
         <v>201</v>
       </c>
@@ -5928,7 +6042,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="199" spans="1:5" ht="45">
+    <row r="199" spans="1:5" ht="45" hidden="1">
       <c r="A199" s="1" t="s">
         <v>202</v>
       </c>
@@ -5945,7 +6059,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="200" spans="1:5" ht="30">
+    <row r="200" spans="1:5" ht="30" hidden="1">
       <c r="A200" s="1" t="s">
         <v>203</v>
       </c>
@@ -5962,7 +6076,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="201" spans="1:5" ht="45">
+    <row r="201" spans="1:5" ht="45" hidden="1">
       <c r="A201" s="1" t="s">
         <v>204</v>
       </c>
@@ -5979,7 +6093,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="202" spans="1:5" ht="45">
+    <row r="202" spans="1:5" ht="45" hidden="1">
       <c r="A202" s="1" t="s">
         <v>205</v>
       </c>
@@ -5996,7 +6110,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="203" spans="1:5" ht="45">
+    <row r="203" spans="1:5" ht="45" hidden="1">
       <c r="A203" s="1" t="s">
         <v>206</v>
       </c>
@@ -6013,7 +6127,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="204" spans="1:5" ht="45">
+    <row r="204" spans="1:5" ht="45" hidden="1">
       <c r="A204" s="1" t="s">
         <v>207</v>
       </c>
@@ -6030,7 +6144,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="205" spans="1:5" ht="30">
+    <row r="205" spans="1:5" ht="30" hidden="1">
       <c r="A205" s="1" t="s">
         <v>208</v>
       </c>
@@ -6047,7 +6161,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="206" spans="1:5" ht="30">
+    <row r="206" spans="1:5" ht="30" hidden="1">
       <c r="A206" s="1" t="s">
         <v>209</v>
       </c>
@@ -6064,7 +6178,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="207" spans="1:5" ht="45">
+    <row r="207" spans="1:5" ht="45" hidden="1">
       <c r="A207" s="1" t="s">
         <v>210</v>
       </c>
@@ -6081,7 +6195,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="208" spans="1:5" ht="60">
+    <row r="208" spans="1:5" ht="60" hidden="1">
       <c r="A208" s="1" t="s">
         <v>211</v>
       </c>
@@ -6098,7 +6212,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="209" spans="1:5">
+    <row r="209" spans="1:5" hidden="1">
       <c r="A209" s="1" t="s">
         <v>212</v>
       </c>
@@ -6115,7 +6229,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="210" spans="1:5" ht="60">
+    <row r="210" spans="1:5" ht="60" hidden="1">
       <c r="A210" s="1" t="s">
         <v>213</v>
       </c>
@@ -6132,7 +6246,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="211" spans="1:5">
+    <row r="211" spans="1:5" hidden="1">
       <c r="A211" s="1" t="s">
         <v>214</v>
       </c>
@@ -6149,7 +6263,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="212" spans="1:5" ht="30">
+    <row r="212" spans="1:5" ht="30" hidden="1">
       <c r="A212" s="1" t="s">
         <v>215</v>
       </c>
@@ -6166,7 +6280,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="30">
+    <row r="213" spans="1:5" ht="30" hidden="1">
       <c r="A213" s="1" t="s">
         <v>216</v>
       </c>
@@ -6183,7 +6297,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="45">
+    <row r="214" spans="1:5" ht="45" hidden="1">
       <c r="A214" s="1" t="s">
         <v>217</v>
       </c>
@@ -6200,7 +6314,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="45">
+    <row r="215" spans="1:5" ht="45" hidden="1">
       <c r="A215" s="1" t="s">
         <v>218</v>
       </c>
@@ -6217,7 +6331,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="216" spans="1:5" ht="30">
+    <row r="216" spans="1:5" ht="30" hidden="1">
       <c r="A216" s="1" t="s">
         <v>219</v>
       </c>
@@ -6234,7 +6348,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="217" spans="1:5" ht="30">
+    <row r="217" spans="1:5" ht="30" hidden="1">
       <c r="A217" s="1" t="s">
         <v>220</v>
       </c>
@@ -6251,7 +6365,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="218" spans="1:5" ht="30">
+    <row r="218" spans="1:5" ht="30" hidden="1">
       <c r="A218" s="1" t="s">
         <v>221</v>
       </c>
@@ -6268,7 +6382,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="30">
+    <row r="219" spans="1:5" ht="30" hidden="1">
       <c r="A219" s="1" t="s">
         <v>222</v>
       </c>
@@ -6285,7 +6399,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="45">
+    <row r="220" spans="1:5" ht="45" hidden="1">
       <c r="A220" s="1" t="s">
         <v>223</v>
       </c>
@@ -6302,7 +6416,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="30">
+    <row r="221" spans="1:5" ht="30" hidden="1">
       <c r="A221" s="1" t="s">
         <v>224</v>
       </c>
@@ -6319,7 +6433,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="222" spans="1:5">
+    <row r="222" spans="1:5" hidden="1">
       <c r="A222" s="1" t="s">
         <v>225</v>
       </c>
@@ -6336,7 +6450,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="30">
+    <row r="223" spans="1:5" ht="30" hidden="1">
       <c r="A223" s="1" t="s">
         <v>226</v>
       </c>
@@ -6353,7 +6467,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="224" spans="1:5">
+    <row r="224" spans="1:5" hidden="1">
       <c r="A224" s="1" t="s">
         <v>227</v>
       </c>
@@ -6370,7 +6484,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="225" spans="1:5" ht="30">
+    <row r="225" spans="1:5" ht="30" hidden="1">
       <c r="A225" s="1" t="s">
         <v>228</v>
       </c>
@@ -6387,7 +6501,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="226" spans="1:5" ht="30">
+    <row r="226" spans="1:5" ht="30" hidden="1">
       <c r="A226" s="1" t="s">
         <v>229</v>
       </c>
@@ -6404,7 +6518,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="227" spans="1:5">
+    <row r="227" spans="1:5" hidden="1">
       <c r="A227" s="1" t="s">
         <v>230</v>
       </c>
@@ -6421,7 +6535,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="228" spans="1:5">
+    <row r="228" spans="1:5" hidden="1">
       <c r="A228" s="1" t="s">
         <v>231</v>
       </c>
@@ -6438,7 +6552,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="229" spans="1:5">
+    <row r="229" spans="1:5" hidden="1">
       <c r="A229" s="1" t="s">
         <v>232</v>
       </c>
@@ -6455,7 +6569,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="230" spans="1:5">
+    <row r="230" spans="1:5" hidden="1">
       <c r="A230" s="1" t="s">
         <v>233</v>
       </c>
@@ -6472,7 +6586,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="231" spans="1:5">
+    <row r="231" spans="1:5" hidden="1">
       <c r="A231" s="1" t="s">
         <v>234</v>
       </c>
@@ -6489,7 +6603,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="232" spans="1:5">
+    <row r="232" spans="1:5" hidden="1">
       <c r="A232" s="1" t="s">
         <v>235</v>
       </c>
@@ -6506,7 +6620,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="233" spans="1:5">
+    <row r="233" spans="1:5" hidden="1">
       <c r="A233" s="1" t="s">
         <v>236</v>
       </c>
@@ -6523,7 +6637,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="234" spans="1:5">
+    <row r="234" spans="1:5" hidden="1">
       <c r="A234" s="1" t="s">
         <v>237</v>
       </c>
@@ -6540,7 +6654,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="235" spans="1:5">
+    <row r="235" spans="1:5" hidden="1">
       <c r="A235" s="1" t="s">
         <v>238</v>
       </c>
@@ -6557,7 +6671,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="236" spans="1:5">
+    <row r="236" spans="1:5" hidden="1">
       <c r="A236" s="1" t="s">
         <v>239</v>
       </c>
@@ -6574,7 +6688,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="237" spans="1:5">
+    <row r="237" spans="1:5" hidden="1">
       <c r="A237" s="1" t="s">
         <v>240</v>
       </c>
@@ -6591,7 +6705,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="238" spans="1:5">
+    <row r="238" spans="1:5" hidden="1">
       <c r="A238" s="1" t="s">
         <v>241</v>
       </c>
@@ -6608,7 +6722,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="239" spans="1:5">
+    <row r="239" spans="1:5" hidden="1">
       <c r="A239" s="1" t="s">
         <v>242</v>
       </c>
@@ -6625,7 +6739,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="240" spans="1:5">
+    <row r="240" spans="1:5" hidden="1">
       <c r="A240" s="1" t="s">
         <v>243</v>
       </c>
@@ -6642,7 +6756,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="241" spans="1:5">
+    <row r="241" spans="1:5" hidden="1">
       <c r="A241" s="1" t="s">
         <v>244</v>
       </c>
@@ -6659,7 +6773,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="242" spans="1:5">
+    <row r="242" spans="1:5" hidden="1">
       <c r="A242" s="1" t="s">
         <v>245</v>
       </c>
@@ -6676,7 +6790,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="243" spans="1:5">
+    <row r="243" spans="1:5" hidden="1">
       <c r="A243" s="1" t="s">
         <v>246</v>
       </c>
@@ -6693,7 +6807,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="244" spans="1:5">
+    <row r="244" spans="1:5" hidden="1">
       <c r="A244" s="1" t="s">
         <v>247</v>
       </c>
@@ -6710,7 +6824,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="245" spans="1:5">
+    <row r="245" spans="1:5" hidden="1">
       <c r="A245" s="1" t="s">
         <v>248</v>
       </c>
@@ -6727,7 +6841,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="246" spans="1:5">
+    <row r="246" spans="1:5" hidden="1">
       <c r="A246" s="1" t="s">
         <v>249</v>
       </c>
@@ -6744,7 +6858,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="247" spans="1:5">
+    <row r="247" spans="1:5" hidden="1">
       <c r="A247" s="1" t="s">
         <v>250</v>
       </c>
@@ -6761,7 +6875,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="248" spans="1:5" ht="75">
+    <row r="248" spans="1:5" ht="75" hidden="1">
       <c r="A248" s="1" t="s">
         <v>251</v>
       </c>
@@ -6778,7 +6892,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="249" spans="1:5">
+    <row r="249" spans="1:5" hidden="1">
       <c r="A249" s="1" t="s">
         <v>252</v>
       </c>
@@ -6795,7 +6909,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="250" spans="1:5">
+    <row r="250" spans="1:5" hidden="1">
       <c r="A250" s="1" t="s">
         <v>253</v>
       </c>
@@ -6812,7 +6926,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="251" spans="1:5">
+    <row r="251" spans="1:5" hidden="1">
       <c r="A251" s="1" t="s">
         <v>254</v>
       </c>
@@ -6829,7 +6943,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="252" spans="1:5">
+    <row r="252" spans="1:5" hidden="1">
       <c r="A252" s="1" t="s">
         <v>255</v>
       </c>
@@ -6846,7 +6960,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="253" spans="1:5">
+    <row r="253" spans="1:5" hidden="1">
       <c r="A253" s="1" t="s">
         <v>256</v>
       </c>
@@ -6863,7 +6977,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="254" spans="1:5">
+    <row r="254" spans="1:5" hidden="1">
       <c r="A254" s="1" t="s">
         <v>238</v>
       </c>
@@ -6880,7 +6994,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="255" spans="1:5" ht="30">
+    <row r="255" spans="1:5" ht="30" hidden="1">
       <c r="A255" s="1" t="s">
         <v>257</v>
       </c>
@@ -6897,7 +7011,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="256" spans="1:5">
+    <row r="256" spans="1:5" hidden="1">
       <c r="A256" s="1" t="s">
         <v>258</v>
       </c>
@@ -6914,7 +7028,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="257" spans="1:5">
+    <row r="257" spans="1:5" hidden="1">
       <c r="A257" s="1" t="s">
         <v>259</v>
       </c>
@@ -6931,7 +7045,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="258" spans="1:5">
+    <row r="258" spans="1:5" hidden="1">
       <c r="A258" s="1" t="s">
         <v>260</v>
       </c>
@@ -6948,7 +7062,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="259" spans="1:5">
+    <row r="259" spans="1:5" hidden="1">
       <c r="A259" s="1" t="s">
         <v>261</v>
       </c>
@@ -6965,7 +7079,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="260" spans="1:5" ht="30">
+    <row r="260" spans="1:5" ht="30" hidden="1">
       <c r="A260" s="1" t="s">
         <v>262</v>
       </c>
@@ -6982,7 +7096,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="261" spans="1:5">
+    <row r="261" spans="1:5" hidden="1">
       <c r="A261" s="1" t="s">
         <v>263</v>
       </c>
@@ -7038,7 +7152,7 @@
         <v>266</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>290</v>
@@ -7072,7 +7186,7 @@
         <v>268</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>290</v>
@@ -7089,7 +7203,7 @@
         <v>269</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>290</v>
@@ -7106,7 +7220,7 @@
         <v>270</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>290</v>
@@ -7123,7 +7237,7 @@
         <v>271</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>290</v>
@@ -7157,7 +7271,7 @@
         <v>273</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C271" s="1" t="s">
         <v>290</v>
@@ -7174,7 +7288,7 @@
         <v>274</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>290</v>
@@ -7191,7 +7305,7 @@
         <v>275</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>290</v>
@@ -7242,7 +7356,7 @@
         <v>278</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>290</v>
@@ -7321,6 +7435,293 @@
       <c r="E280" s="1" t="s">
         <v>560</v>
       </c>
+    </row>
+    <row r="281" spans="1:5" hidden="1">
+      <c r="A281" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="B281" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C281" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D281" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E281" s="3" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" hidden="1">
+      <c r="A282" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="B282" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C282" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D282" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E282" s="3" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" hidden="1">
+      <c r="A283" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="B283" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C283" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D283" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E283" s="3" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" ht="30" hidden="1">
+      <c r="A284" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="B284" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C284" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D284" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E284" s="3" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" ht="45" hidden="1">
+      <c r="A285" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="B285" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C285" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D285" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E285" s="3" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" hidden="1">
+      <c r="A286" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="B286" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D286" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E286" s="2" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" hidden="1">
+      <c r="A287" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="B287" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C287" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D287" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E287" s="3" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" hidden="1">
+      <c r="A288" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="B288" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C288" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D288" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E288" s="3" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" ht="45" hidden="1">
+      <c r="A289" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="B289" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C289" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D289" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E289" s="3" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" hidden="1">
+      <c r="A290" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="B290" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C290" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D290" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E290" s="3" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" hidden="1">
+      <c r="A291" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="B291" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C291" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D291" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E291" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" ht="105" hidden="1">
+      <c r="A292" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="B292" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C292" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D292" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="E292" s="3" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" ht="45" hidden="1">
+      <c r="A293" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="B293" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C293" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D293" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E293" s="3" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" ht="30" hidden="1">
+      <c r="A294" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="B294" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D294" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E294" s="2" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" ht="30" hidden="1">
+      <c r="A295" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="B295" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D295" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E295" s="2" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" ht="90" hidden="1">
+      <c r="A296" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="B296" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C296" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D296" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E296" s="3" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" hidden="1">
+      <c r="A297" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="B297" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C297" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D297" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E297" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>